<commit_message>
Added a bit of data
</commit_message>
<xml_diff>
--- a/Full_dataset from STATA.xlsx
+++ b/Full_dataset from STATA.xlsx
@@ -33598,6 +33598,9 @@
       <c r="G876" s="1">
         <v>46.0</v>
       </c>
+      <c r="H876" s="2">
+        <v>-4.0</v>
+      </c>
       <c r="I876" s="1">
         <v>5.276674615217862E10</v>
       </c>
@@ -33627,6 +33630,9 @@
       <c r="E877" s="1">
         <v>4.114814</v>
       </c>
+      <c r="H877" s="2">
+        <v>-4.0</v>
+      </c>
       <c r="I877" s="1">
         <v>5.7730380599528465E10</v>
       </c>
@@ -33650,6 +33656,9 @@
       <c r="E878" s="1">
         <v>4.056373</v>
       </c>
+      <c r="H878" s="2">
+        <v>-4.0</v>
+      </c>
       <c r="I878" s="1">
         <v>6.49417130573775E10</v>
       </c>
@@ -33676,6 +33685,9 @@
       <c r="G879" s="1">
         <v>51.0</v>
       </c>
+      <c r="H879" s="2">
+        <v>-4.0</v>
+      </c>
       <c r="I879" s="1">
         <v>7.42945082395524E10</v>
       </c>
@@ -33705,6 +33717,9 @@
       <c r="G880" s="1">
         <v>51.0</v>
       </c>
+      <c r="H880" s="2">
+        <v>-4.0</v>
+      </c>
       <c r="I880" s="1">
         <v>5.1772232494854E10</v>
       </c>
@@ -33737,6 +33752,9 @@
       <c r="G881" s="1">
         <v>24.0</v>
       </c>
+      <c r="H881" s="2">
+        <v>-4.0</v>
+      </c>
       <c r="I881" s="1">
         <v>4.502107795532797E10</v>
       </c>
@@ -33769,6 +33787,9 @@
       <c r="G882" s="1">
         <v>0.0</v>
       </c>
+      <c r="H882" s="2">
+        <v>-4.0</v>
+      </c>
       <c r="I882" s="1">
         <v>3.3128480498729603E10</v>
       </c>
@@ -54887,6 +54908,9 @@
       <c r="G1442" s="1">
         <v>54.0</v>
       </c>
+      <c r="H1442" s="2">
+        <v>-7.0</v>
+      </c>
       <c r="I1442" s="1">
         <v>3.506410550083445E10</v>
       </c>
@@ -54919,6 +54943,9 @@
       <c r="G1443" s="1">
         <v>2.0</v>
       </c>
+      <c r="H1443" s="2">
+        <v>-7.0</v>
+      </c>
       <c r="I1443" s="1">
         <v>3.9552513316073425E10</v>
       </c>
@@ -54954,6 +54981,9 @@
       <c r="G1444" s="1">
         <v>298.0</v>
       </c>
+      <c r="H1444" s="2">
+        <v>-7.0</v>
+      </c>
       <c r="I1444" s="1">
         <v>4.542785469325543E10</v>
       </c>
@@ -54989,6 +55019,9 @@
       <c r="G1445" s="1">
         <v>164.0</v>
       </c>
+      <c r="H1445" s="2">
+        <v>-7.0</v>
+      </c>
       <c r="I1445" s="1">
         <v>5.7633255618273094E10</v>
       </c>
@@ -55030,6 +55063,9 @@
       <c r="G1446" s="1">
         <v>16.0</v>
       </c>
+      <c r="H1446" s="2">
+        <v>-7.0</v>
+      </c>
       <c r="I1446" s="1">
         <v>6.6371664817043625E10</v>
       </c>
@@ -55071,6 +55107,9 @@
       <c r="G1447" s="1">
         <v>2.0</v>
       </c>
+      <c r="H1447" s="2">
+        <v>-7.0</v>
+      </c>
       <c r="I1447" s="1">
         <v>7.741442553224516E10</v>
       </c>
@@ -55112,6 +55151,9 @@
       <c r="G1448" s="1">
         <v>168.0</v>
       </c>
+      <c r="H1448" s="2">
+        <v>-7.0</v>
+      </c>
       <c r="I1448" s="1">
         <v>9.913030409912743E10</v>
       </c>
@@ -55153,6 +55195,9 @@
       <c r="G1449" s="1">
         <v>55.0</v>
       </c>
+      <c r="H1449" s="2">
+        <v>-7.0</v>
+      </c>
       <c r="I1449" s="1">
         <v>1.0601465977022217E11</v>
       </c>
@@ -55194,6 +55239,9 @@
       <c r="G1450" s="1">
         <v>151.0</v>
       </c>
+      <c r="H1450" s="2">
+        <v>-7.0</v>
+      </c>
       <c r="I1450" s="1">
         <v>1.1593174969724115E11</v>
       </c>
@@ -55235,6 +55283,9 @@
       <c r="G1451" s="1">
         <v>985.0</v>
       </c>
+      <c r="H1451" s="2">
+        <v>-7.0</v>
+      </c>
       <c r="I1451" s="1">
         <v>1.3553943855970941E11</v>
       </c>
@@ -55273,6 +55324,9 @@
       <c r="G1452" s="1">
         <v>768.0</v>
       </c>
+      <c r="H1452" s="2">
+        <v>-7.0</v>
+      </c>
       <c r="I1452" s="1">
         <v>1.5582000192049164E11</v>
       </c>
@@ -55311,6 +55365,9 @@
       <c r="G1453" s="1">
         <v>313.0</v>
       </c>
+      <c r="H1453" s="2">
+        <v>-7.0</v>
+      </c>
       <c r="I1453" s="1">
         <v>1.7122202511738086E11</v>
       </c>
@@ -55349,6 +55406,9 @@
       <c r="G1454" s="1">
         <v>1062.0</v>
       </c>
+      <c r="H1454" s="2">
+        <v>-7.0</v>
+      </c>
       <c r="I1454" s="1">
         <v>1.8620465292226215E11</v>
       </c>
@@ -55387,6 +55447,9 @@
       <c r="G1455" s="1">
         <v>742.0</v>
       </c>
+      <c r="H1455" s="2">
+        <v>-7.0</v>
+      </c>
       <c r="I1455" s="1">
         <v>1.9324110870953622E11</v>
       </c>
@@ -55425,6 +55488,9 @@
       <c r="G1456" s="1">
         <v>706.0</v>
       </c>
+      <c r="H1456" s="2">
+        <v>-7.0</v>
+      </c>
       <c r="I1456" s="1">
         <v>2.052761721349014E11</v>
       </c>
@@ -55466,6 +55532,9 @@
       <c r="G1457" s="1">
         <v>467.0</v>
       </c>
+      <c r="H1457" s="2">
+        <v>-7.0</v>
+      </c>
       <c r="I1457" s="1">
         <v>2.2377986581518256E11</v>
       </c>
@@ -55506,6 +55575,9 @@
       </c>
       <c r="G1458" s="1">
         <v>335.0</v>
+      </c>
+      <c r="H1458" s="2">
+        <v>-7.0</v>
       </c>
       <c r="I1458" s="1">
         <v>2.452136863691568E11</v>

</xml_diff>